<commit_message>
capex and opex of cooling and ventilation calculated
</commit_message>
<xml_diff>
--- a/projects/test_building/input/ID_Sector.xlsx
+++ b/projects/test_building/input/ID_Sector.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AB12A9-A9CD-124F-A4FC-FCEAF9D1B981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AEF87E-1DD5-F347-BA91-10D3B39C68F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,24 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>Agriculture</t>
-  </si>
-  <si>
-    <t>Industry</t>
-  </si>
-  <si>
     <t>Tertiary</t>
-  </si>
-  <si>
-    <t>Construction</t>
-  </si>
-  <si>
-    <t>Energy</t>
   </si>
   <si>
     <t>Residential</t>
@@ -99,8 +87,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F01526EB-050A-F345-8814-23409122B67A}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0">
-  <autoFilter ref="A1:B7" xr:uid="{F01526EB-050A-F345-8814-23409122B67A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F01526EB-050A-F345-8814-23409122B67A}" name="Table1" displayName="Table1" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3" xr:uid="{F01526EB-050A-F345-8814-23409122B67A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{10BDC833-DD80-084B-B342-398A0CF49EE5}" name="id_sector"/>
     <tableColumn id="2" xr3:uid="{3FE1080A-0BAF-1143-88D1-C39E48F99732}" name="name"/>
@@ -372,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -385,7 +373,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -393,7 +381,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -401,42 +389,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>